<commit_message>
Eerste uses cases. Check ook excel
</commit_message>
<xml_diff>
--- a/Doc/analyse/use_casses.xlsx
+++ b/Doc/analyse/use_casses.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>add organism</t>
   </si>
@@ -395,7 +395,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,20 +436,32 @@
       <c r="A6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Family object in subfamily ipv id
</commit_message>
<xml_diff>
--- a/Doc/analyse/use_casses.xlsx
+++ b/Doc/analyse/use_casses.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitBioDiversity_Oman\ProjectOman\Doc\analyse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectOman\Doc\analyse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12504"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>add organism</t>
   </si>
@@ -68,10 +68,7 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>aanpassen</t>
-  </si>
-  <si>
-    <t>aangepast</t>
+    <t>Eric</t>
   </si>
 </sst>
 </file>
@@ -398,29 +395,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -428,7 +419,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -436,7 +427,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -444,7 +435,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -452,7 +443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -460,7 +451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -468,7 +459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -476,27 +467,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>

</xml_diff>